<commit_message>
0.0.3 add new admin comand 'new_student' problem
</commit_message>
<xml_diff>
--- a/data_base/database structure.xlsx
+++ b/data_base/database structure.xlsx
@@ -6,16 +6,17 @@
   </bookViews>
   <sheets>
     <sheet name="Обзор экспорта" sheetId="1" r:id="rId4"/>
-    <sheet name="Main data base - Основная табли" sheetId="2" r:id="rId5"/>
-    <sheet name="Group 1 - Group 1" sheetId="3" r:id="rId6"/>
-    <sheet name="Group 2 - Group 2" sheetId="4" r:id="rId7"/>
-    <sheet name="Group 3 - Group 3" sheetId="5" r:id="rId8"/>
+    <sheet name="main_data_base - Основная табли" sheetId="2" r:id="rId5"/>
+    <sheet name="names_groups - Id групп и их на" sheetId="3" r:id="rId6"/>
+    <sheet name="group_0 - group_0" sheetId="4" r:id="rId7"/>
+    <sheet name="group_1 - group_1" sheetId="5" r:id="rId8"/>
+    <sheet name="group_2 - group_2" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Документ был экспортирован из Numbers. Каждая таблица была конвертирована в рабочий лист Excel. Все другие объекты на листах Numbers были помещены на отдельные рабочие листы. Имейте в виду, что расчеты формул могут отличаться от расчетов в Excel.</t>
   </si>
@@ -29,31 +30,34 @@
     <t>Название рабочего листа Excel</t>
   </si>
   <si>
-    <t>Main data base</t>
-  </si>
-  <si>
-    <t>Основная таблица по группам</t>
-  </si>
-  <si>
-    <t>Main data base - Основная табли</t>
-  </si>
-  <si>
-    <t>Id PRIMARY KEY</t>
-  </si>
-  <si>
-    <t>group 1 INTEGER</t>
-  </si>
-  <si>
-    <t>group 2 INTEGER</t>
-  </si>
-  <si>
-    <t>group 3 INTEGER</t>
-  </si>
-  <si>
-    <t>group 4 INTEGER</t>
-  </si>
-  <si>
-    <t>group  5 INTEGER</t>
+    <t>main_data_base</t>
+  </si>
+  <si>
+    <t>Основная таблица по группам и студентам (в каких они группах находятся)</t>
+  </si>
+  <si>
+    <t>main_data_base - Основная табли</t>
+  </si>
+  <si>
+    <t>id INTEGER PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>id_telegram INTEGER</t>
+  </si>
+  <si>
+    <t>group_0 INTEGER</t>
+  </si>
+  <si>
+    <t>group_1 INTEGER</t>
+  </si>
+  <si>
+    <t>group_2 INTEGER</t>
+  </si>
+  <si>
+    <t>group_3 INTEGER</t>
+  </si>
+  <si>
+    <t>group_4 INTEGER</t>
   </si>
   <si>
     <t>group (и т.д. до 20 например)</t>
@@ -62,16 +66,46 @@
     <t>Id студента в таблице (и в остальных таблицах будет id братья из этой таблицы)</t>
   </si>
   <si>
+    <t>Телеграм id студента (можно менять при смене аккаунта) а так же по нему проводится поиск студента</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 - если относится к данной группе        0 - не относится к данной группе </t>
   </si>
   <si>
+    <t xml:space="preserve">Столбцы должны создаваться только тогда, когда группа создаётся </t>
+  </si>
+  <si>
     <t>Будет проверяться в какой группе студент и переводить в таблицы тех групп, где этот студент присутствует</t>
   </si>
   <si>
-    <t>Group 1</t>
-  </si>
-  <si>
-    <t>Group 1 - Group 1</t>
+    <t>names_groups</t>
+  </si>
+  <si>
+    <t>Id групп и их названия</t>
+  </si>
+  <si>
+    <t>names_groups - Id групп и их на</t>
+  </si>
+  <si>
+    <t>num_group INTEGER PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>name_group TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id группы </t>
+  </si>
+  <si>
+    <t>Название группы</t>
+  </si>
+  <si>
+    <t>group_0</t>
+  </si>
+  <si>
+    <t>group_0 - group_0</t>
+  </si>
+  <si>
+    <t>id PRIMARY KEY</t>
   </si>
   <si>
     <t>num_student_card TEXT</t>
@@ -80,9 +114,6 @@
     <t>name_student TEXT</t>
   </si>
   <si>
-    <t>id_telegram INTEGER</t>
-  </si>
-  <si>
     <t>Status INTEGER</t>
   </si>
   <si>
@@ -104,37 +135,40 @@
     <t>datetime т.д. (номера вопросов - номер столбца) создаются автоматически при новых вопросах</t>
   </si>
   <si>
+    <t>id студента в таблице (берётся из Main data base)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номе зачётки студента </t>
+  </si>
+  <si>
+    <t>ФИО студента</t>
+  </si>
+  <si>
+    <t>Телеграм id студента (можно менять при смене аккаунта)</t>
+  </si>
+  <si>
+    <t>Не заблокировал ли студент бота (1 - бот работает, 0 - бот заблокирован)</t>
+  </si>
+  <si>
+    <t>Ответ на вопрос (Да | Нет | Другой ответ, который написал студент)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В какую дату и  время ответил студент </t>
+  </si>
+  <si>
+    <t>group_1</t>
+  </si>
+  <si>
+    <t>group_1 - group_1</t>
+  </si>
+  <si>
     <t>Id студента в таблице (берётся из Main data base)</t>
   </si>
   <si>
-    <t xml:space="preserve">Номе зачётки студента </t>
-  </si>
-  <si>
-    <t>ФИО студента</t>
-  </si>
-  <si>
-    <t>Телеграм id студента (можно менять при смене аккаунта)</t>
-  </si>
-  <si>
-    <t>Не заблокировал ли студент бота (1 - бот работает, 0 - бот заблокирован)</t>
-  </si>
-  <si>
-    <t>Ответ на вопрос (Да | Нет | Другой ответ, который написал студент)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В какую дату и  время ответил студент </t>
-  </si>
-  <si>
-    <t>Group 2</t>
-  </si>
-  <si>
-    <t>Group 2 - Group 2</t>
-  </si>
-  <si>
-    <t>Group 3</t>
-  </si>
-  <si>
-    <t>Group 3 - Group 3</t>
+    <t>group_2</t>
+  </si>
+  <si>
+    <t>group_2 - group_2</t>
   </si>
 </sst>
 </file>
@@ -324,7 +358,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -373,10 +407,16 @@
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1515,7 +1555,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1523,15 +1563,15 @@
     <row r="12">
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1539,15 +1579,15 @@
     <row r="14">
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="3">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1555,10 +1595,26 @@
     <row r="16">
       <c r="B16" s="4"/>
       <c r="C16" t="s" s="4">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>39</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1566,10 +1622,11 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Main data base - Основная табли'!R2C1" tooltip="" display="Main data base - Основная табли"/>
-    <hyperlink ref="D12" location="'Group 1 - Group 1'!R2C1" tooltip="" display="Group 1 - Group 1"/>
-    <hyperlink ref="D14" location="'Group 2 - Group 2'!R2C1" tooltip="" display="Group 2 - Group 2"/>
-    <hyperlink ref="D16" location="'Group 3 - Group 3'!R2C1" tooltip="" display="Group 3 - Group 3"/>
+    <hyperlink ref="D10" location="'main_data_base - Основная табли'!R2C1" tooltip="" display="main_data_base - Основная табли"/>
+    <hyperlink ref="D12" location="'names_groups - Id групп и их на'!R2C1" tooltip="" display="names_groups - Id групп и их на"/>
+    <hyperlink ref="D14" location="'group_0 - group_0'!R2C1" tooltip="" display="group_0 - group_0"/>
+    <hyperlink ref="D16" location="'group_1 - group_1'!R2C1" tooltip="" display="group_1 - group_1"/>
+    <hyperlink ref="D18" location="'group_2 - group_2'!R2C1" tooltip="" display="group_2 - group_2"/>
   </hyperlinks>
 </worksheet>
 </file>
@@ -1579,7 +1636,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1587,8 +1644,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="16.3516" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="24.4297" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.2109" style="6" customWidth="1"/>
+    <col min="3" max="9" width="16.3516" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1602,6 +1661,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" ht="32.25" customHeight="1">
       <c r="A2" t="s" s="8">
@@ -1625,117 +1685,133 @@
       <c r="G2" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" ht="80.25" customHeight="1">
       <c r="A3" t="s" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s" s="11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s" s="12">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s" s="12">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" ht="68.05" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="C4" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" ht="116.05" customHeight="1">
-      <c r="A7" t="s" s="17">
-        <v>16</v>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" ht="68.05" customHeight="1">
+      <c r="A7" t="s" s="18">
+        <v>19</v>
       </c>
       <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1747,6 +1823,123 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="32.7109" style="19" customWidth="1"/>
+    <col min="2" max="5" width="16.3516" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
@@ -1755,17 +1948,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.1172" style="18" customWidth="1"/>
-    <col min="2" max="2" width="21.1172" style="18" customWidth="1"/>
-    <col min="3" max="3" width="17.5781" style="18" customWidth="1"/>
-    <col min="4" max="4" width="19.3906" style="18" customWidth="1"/>
-    <col min="5" max="11" width="16.3516" style="18" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="18" customWidth="1"/>
+    <col min="1" max="1" width="16.1172" style="20" customWidth="1"/>
+    <col min="2" max="2" width="21.1172" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.5781" style="20" customWidth="1"/>
+    <col min="4" max="4" width="19.3906" style="20" customWidth="1"/>
+    <col min="5" max="11" width="16.3516" style="20" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1780,66 +1973,66 @@
     </row>
     <row r="2" ht="104.25" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s" s="8">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s" s="8">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s" s="8">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s" s="8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s" s="8">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="8">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="56.25" customHeight="1">
       <c r="A3" t="s" s="10">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="11">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="12">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="12">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s" s="12">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s" s="12">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s" s="12">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1847,262 +2040,262 @@
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2110,376 +2303,6 @@
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:K23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="11" width="16.3516" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" ht="104.25" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s" s="8">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" ht="56.25" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s" s="12">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s" s="12">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="12">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s" s="12">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s" s="12">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s" s="12">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s" s="12">
-        <v>35</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2499,13 +2322,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="11" width="16.3516" style="20" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="20" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="21" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2520,66 +2343,66 @@
     </row>
     <row r="2" ht="104.25" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s" s="8">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s" s="8">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s" s="8">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s" s="8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s" s="8">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="8">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="56.25" customHeight="1">
       <c r="A3" t="s" s="10">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s" s="11">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="12">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="12">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s" s="12">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s" s="12">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s" s="12">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -2587,262 +2410,632 @@
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="11" width="16.3516" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" ht="104.25" customHeight="1">
+      <c r="A2" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s" s="8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" ht="56.25" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s" s="11">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="12">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s" s="12">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s" s="12">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s" s="12">
+        <v>45</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>